<commit_message>
Mod 2 Final Project -Complete v2-JMI.ipynb ready as final. Blog post published but still needs fixing.
</commit_message>
<xml_diff>
--- a/Exported csv/table_H4_test_results.xlsx
+++ b/Exported csv/table_H4_test_results.xlsx
@@ -491,24 +491,24 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A vs B</t>
+          <t>A vs. B:</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>mannwhitneyu</t>
+          <t>ttest_ind</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Hypothesis sig.</t>
+          <t>Hypothsis sig</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>77366.5</v>
+        <v>4.9876</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0002271025107896975</v>
+        <v>3.902807969589616e-07</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>

</xml_diff>